<commit_message>
Look lots of data
</commit_message>
<xml_diff>
--- a/synonym_table.xlsx
+++ b/synonym_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejayb\HealthDataAnalytics\Proj2\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E6515DE-F00A-4E20-8F11-8A6827538198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B53F87A-F4C0-47B8-90BD-56687B52FDDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0BBF9582-3669-432E-A97E-018BFA67D8A8}"/>
   </bookViews>
@@ -147,13 +147,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,10 +170,39 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -176,14 +211,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -194,6 +305,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0253A64D-ACDD-4228-880B-700E29EF5F52}" name="Table1" displayName="Table1" ref="A1:B21" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="3">
+  <autoFilter ref="A1:B21" xr:uid="{6894D092-89E1-45B5-AB1C-FCDA9CD02A59}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{79030C5C-4C5D-489F-9C7A-308118D470B4}" name="Vital Sign" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{7388CA5C-85F4-4990-9D2C-31908B47F595}" name="Synonyms and Indicators" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -496,166 +618,175 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="B17" s="5"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>